<commit_message>
feat: Libary Excel Export
</commit_message>
<xml_diff>
--- a/Sereno.Documentation.Dal/FileAccess/DocumentsTemplate.xlsx
+++ b/Sereno.Documentation.Dal/FileAccess/DocumentsTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Privat\Sereno\Sereno.Documentation.Dal\FileAccess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8E2377-F6F8-496D-9446-D1C377FFC265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D353A-8BA2-4359-A1EF-39711378615C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46630" yWindow="4900" windowWidth="28800" windowHeight="15380" xr2:uid="{CAA557EC-6762-47A3-90D7-79230F151C5E}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="21600" windowHeight="12773" xr2:uid="{CAA557EC-6762-47A3-90D7-79230F151C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Dokumente" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Pfad</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Author</t>
   </si>
@@ -49,6 +46,21 @@
   </si>
   <si>
     <t>IT Dokumentation | Dokumente</t>
+  </si>
+  <si>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>Dokumentation Titel</t>
+  </si>
+  <si>
+    <t>Datei Pfad</t>
+  </si>
+  <si>
+    <t>Bibliothek Pfad</t>
+  </si>
+  <si>
+    <t>D:\Doku\Produkte\Outlook</t>
   </si>
 </sst>
 </file>
@@ -99,7 +111,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor theme="6"/>
       </patternFill>
     </fill>
@@ -120,19 +132,6 @@
       <top style="thin">
         <color theme="6"/>
       </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -144,6 +143,17 @@
       <top style="thin">
         <color theme="6"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
       <bottom style="thin">
         <color theme="6"/>
       </bottom>
@@ -157,7 +167,9 @@
       <top style="thin">
         <color theme="6"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -168,11 +180,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,38 +499,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7B32BD-0DE2-4D9E-A99C-0B52E5E685A2}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.9296875" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="102.81640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="55.81640625" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="50.86328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="55.796875" style="3" customWidth="1"/>
+    <col min="3" max="4" width="95.3984375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.9296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="16.899999999999999" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>